<commit_message>
Thu Nov 30 16:55:13 CST 2023
</commit_message>
<xml_diff>
--- a/data/nutrion.value.xlsx
+++ b/data/nutrion.value.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\a-document\sequencing_center_desktop\yanglab\中农教务\南方地力提升 保密i项目\肉牛生长营养\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\a-document\github\cattle_nutrition\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,12 +14,12 @@
   <sheets>
     <sheet name="营养表1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="148">
   <si>
     <t>0,16</t>
   </si>
@@ -28,446 +28,448 @@
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>89..1</t>
+    <t>Calcium</t>
+  </si>
+  <si>
+    <t>Phosphorus</t>
+  </si>
+  <si>
+    <t>Fermentable organic matter</t>
+  </si>
+  <si>
+    <t>Barley seedlings</t>
+  </si>
+  <si>
+    <t>sweet potato vine</t>
+  </si>
+  <si>
+    <t>Ryegrass</t>
+  </si>
+  <si>
+    <t>alfalfa</t>
+  </si>
+  <si>
+    <t>satawang</t>
+  </si>
+  <si>
+    <t>Elephant grass</t>
+  </si>
+  <si>
+    <t>weed</t>
+  </si>
+  <si>
+    <t>sweet potato</t>
+  </si>
+  <si>
+    <t>carrot</t>
+  </si>
+  <si>
+    <t>potato</t>
+  </si>
+  <si>
+    <t>beet</t>
+  </si>
+  <si>
+    <t>Dried beets</t>
+  </si>
+  <si>
+    <t>rutabagas</t>
+  </si>
+  <si>
+    <t>corn</t>
+  </si>
+  <si>
+    <t>Sorghum</t>
+  </si>
+  <si>
+    <t>barley</t>
+  </si>
+  <si>
+    <t>indica rice</t>
+  </si>
+  <si>
+    <t>oat</t>
+  </si>
+  <si>
+    <t>wheat</t>
+  </si>
+  <si>
+    <t>grease</t>
+  </si>
+  <si>
+    <t>wheat bran</t>
+  </si>
+  <si>
+    <t>corn husks</t>
+  </si>
+  <si>
+    <t>rice bran</t>
+  </si>
+  <si>
+    <t>sorghum bran</t>
+  </si>
+  <si>
+    <t>second powder</t>
+  </si>
+  <si>
+    <t>soybean hulls</t>
+  </si>
+  <si>
+    <t>cake</t>
+  </si>
+  <si>
+    <t>soybean meal</t>
+  </si>
+  <si>
+    <t>kenaf cake</t>
+  </si>
+  <si>
+    <t>Cotton kernel cake</t>
+  </si>
+  <si>
+    <t>cotton cypress</t>
+  </si>
+  <si>
+    <t>Di Ke Xiang Japanese Cake</t>
+  </si>
+  <si>
+    <t>Go bright sunflower cake</t>
+  </si>
+  <si>
+    <t>Rapeseed cake</t>
+  </si>
+  <si>
+    <t>Rapeseed meal</t>
+  </si>
+  <si>
+    <t>peanut cake</t>
+  </si>
+  <si>
+    <t>Corn germ cake</t>
+  </si>
+  <si>
+    <t>Rice bran cake</t>
+  </si>
+  <si>
+    <t>sesame cake</t>
+  </si>
+  <si>
+    <t>Tofu dregs</t>
+  </si>
+  <si>
+    <t>Corn meal residue</t>
+  </si>
+  <si>
+    <t>Potato flour residue</t>
+  </si>
+  <si>
+    <t>Pea flour residue</t>
+  </si>
+  <si>
+    <t>Mung bean flour residue</t>
+  </si>
+  <si>
+    <t>Tapioca flour residue</t>
+  </si>
+  <si>
+    <t>Soy sauce residue</t>
+  </si>
+  <si>
+    <t>corn trough</t>
+  </si>
+  <si>
+    <t>Sweet potato dry wine tank</t>
+  </si>
+  <si>
+    <t>Grain bran distiller's grains</t>
+  </si>
+  <si>
+    <t>Rice distiller's grains</t>
+  </si>
+  <si>
+    <t>Sorghum distiller's grains</t>
+  </si>
+  <si>
+    <t>Beer! Liquor lees</t>
+  </si>
+  <si>
+    <t>beet pulp</t>
+  </si>
+  <si>
+    <t>Orange pulp</t>
+  </si>
+  <si>
+    <t>Apple pomace</t>
+  </si>
+  <si>
+    <t>corn silage</t>
+  </si>
+  <si>
+    <t>Alfalfa silage</t>
+  </si>
+  <si>
+    <t>beet leaf silage</t>
+  </si>
+  <si>
+    <t>Leymus chinensis</t>
+  </si>
+  <si>
+    <t>alfalfa hay</t>
+  </si>
+  <si>
+    <t>wild hay</t>
+  </si>
+  <si>
+    <t>Alkali grass</t>
+  </si>
+  <si>
+    <t>Corn stalks</t>
+  </si>
+  <si>
+    <t>wheat straw</t>
+  </si>
+  <si>
+    <t>straw</t>
+  </si>
+  <si>
+    <t>cereal grass</t>
+  </si>
+  <si>
+    <t>sweet potato seedlings</t>
+  </si>
+  <si>
+    <t>peanut seedlings</t>
+  </si>
+  <si>
+    <t>大麦苗</t>
+  </si>
+  <si>
+    <t>甘薯藤</t>
+  </si>
+  <si>
+    <t>黑麦草</t>
+  </si>
+  <si>
+    <t>苜蓿</t>
+  </si>
+  <si>
+    <t>沙打旺</t>
+  </si>
+  <si>
+    <t>象草</t>
+  </si>
+  <si>
+    <t>野草</t>
+  </si>
+  <si>
+    <t>甘薯</t>
+  </si>
+  <si>
+    <t>胡萝卜</t>
+  </si>
+  <si>
+    <t>马铃薯</t>
+  </si>
+  <si>
+    <t>甜菜</t>
+  </si>
+  <si>
+    <t>甜菜丝干</t>
+  </si>
+  <si>
+    <t>芜菁甘蓝</t>
+  </si>
+  <si>
+    <t>玉米</t>
+  </si>
+  <si>
+    <t>高粱</t>
+  </si>
+  <si>
+    <t>大麦</t>
+  </si>
+  <si>
+    <t>籼稻谷</t>
+  </si>
+  <si>
+    <t>燕麦</t>
+  </si>
+  <si>
+    <t>小麦</t>
+  </si>
+  <si>
+    <t>油脂</t>
+  </si>
+  <si>
+    <t>小麦麸</t>
+  </si>
+  <si>
+    <t>玉米皮</t>
+  </si>
+  <si>
+    <t>米糠</t>
+  </si>
+  <si>
+    <t>高粱糠</t>
+  </si>
+  <si>
+    <t>次粉</t>
+  </si>
+  <si>
+    <t>大豆皮</t>
+  </si>
+  <si>
+    <t>豆饼</t>
+  </si>
+  <si>
+    <t>豆粕</t>
+  </si>
+  <si>
+    <t>红麻饼</t>
+  </si>
+  <si>
+    <t>棉仁饼</t>
+  </si>
+  <si>
+    <t>棉仁柏</t>
+  </si>
+  <si>
+    <t>蒂壳向日资饼</t>
+  </si>
+  <si>
+    <t>去亮向日葵饼</t>
+  </si>
+  <si>
+    <t>菜籽饼</t>
+  </si>
+  <si>
+    <t>菜籽粕</t>
+  </si>
+  <si>
+    <t>花生饼</t>
+  </si>
+  <si>
+    <t>玉米胚芽饼</t>
+  </si>
+  <si>
+    <t>米糠饼</t>
+  </si>
+  <si>
+    <t>芝麻饼</t>
+  </si>
+  <si>
+    <t>豆腐渣</t>
+  </si>
+  <si>
+    <t>玉米粉渣</t>
+  </si>
+  <si>
+    <t>土豆粉渣</t>
+  </si>
+  <si>
+    <t>豌豆粉渣</t>
+  </si>
+  <si>
+    <t>绿豆粉渣</t>
+  </si>
+  <si>
+    <t>木薯粉渣</t>
+  </si>
+  <si>
+    <t>酱油渣</t>
+  </si>
+  <si>
+    <t>玉米酒槽</t>
+  </si>
+  <si>
+    <t>红薯干酒槽</t>
+  </si>
+  <si>
+    <t>谷糠酒糟</t>
+  </si>
+  <si>
+    <t>大米酒糟</t>
+  </si>
+  <si>
+    <t>高粱酒糟</t>
+  </si>
+  <si>
+    <t>啤!酒糟</t>
+  </si>
+  <si>
+    <t>甜菜渣</t>
+  </si>
+  <si>
+    <t>橘子渣</t>
+  </si>
+  <si>
+    <t>苹果渣</t>
+  </si>
+  <si>
+    <t>玉米青贮</t>
+  </si>
+  <si>
+    <t>苜蓿青贮</t>
+  </si>
+  <si>
+    <t>甜菜叶青贮</t>
+  </si>
+  <si>
+    <t>羊草</t>
+  </si>
+  <si>
+    <t>苜蓿干草</t>
+  </si>
+  <si>
+    <t>野干草</t>
+  </si>
+  <si>
+    <t>碱草</t>
+  </si>
+  <si>
+    <t>玉米秸秆</t>
+  </si>
+  <si>
+    <t>小麦秸秆</t>
+  </si>
+  <si>
+    <t>稻草</t>
+  </si>
+  <si>
+    <t>谷草</t>
+  </si>
+  <si>
+    <t>甘薯秧</t>
+  </si>
+  <si>
+    <t>花生秧</t>
+  </si>
+  <si>
+    <t>materia</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
   <si>
-    <t>Raw materials</t>
-  </si>
-  <si>
-    <t>Dry matter</t>
-  </si>
-  <si>
-    <t>Comprehensive net energy</t>
-  </si>
-  <si>
-    <t>Crude protein</t>
-  </si>
-  <si>
-    <t>Calcium</t>
-  </si>
-  <si>
-    <t>Phosphorus</t>
-  </si>
-  <si>
-    <t>Fermentable organic matter</t>
-  </si>
-  <si>
-    <t>Barley seedlings</t>
-  </si>
-  <si>
-    <t>sweet potato vine</t>
-  </si>
-  <si>
-    <t>Ryegrass</t>
-  </si>
-  <si>
-    <t>alfalfa</t>
-  </si>
-  <si>
-    <t>satawang</t>
-  </si>
-  <si>
-    <t>Elephant grass</t>
-  </si>
-  <si>
-    <t>weed</t>
-  </si>
-  <si>
-    <t>sweet potato</t>
-  </si>
-  <si>
-    <t>carrot</t>
-  </si>
-  <si>
-    <t>potato</t>
-  </si>
-  <si>
-    <t>beet</t>
-  </si>
-  <si>
-    <t>Dried beets</t>
-  </si>
-  <si>
-    <t>rutabagas</t>
-  </si>
-  <si>
-    <t>corn</t>
-  </si>
-  <si>
-    <t>Sorghum</t>
-  </si>
-  <si>
-    <t>barley</t>
-  </si>
-  <si>
-    <t>indica rice</t>
-  </si>
-  <si>
-    <t>oat</t>
-  </si>
-  <si>
-    <t>wheat</t>
-  </si>
-  <si>
-    <t>grease</t>
-  </si>
-  <si>
-    <t>wheat bran</t>
-  </si>
-  <si>
-    <t>corn husks</t>
-  </si>
-  <si>
-    <t>rice bran</t>
-  </si>
-  <si>
-    <t>sorghum bran</t>
-  </si>
-  <si>
-    <t>second powder</t>
-  </si>
-  <si>
-    <t>soybean hulls</t>
-  </si>
-  <si>
-    <t>cake</t>
-  </si>
-  <si>
-    <t>soybean meal</t>
-  </si>
-  <si>
-    <t>kenaf cake</t>
-  </si>
-  <si>
-    <t>Chenzi cake</t>
-  </si>
-  <si>
-    <t>Cotton kernel cake</t>
-  </si>
-  <si>
-    <t>cotton cypress</t>
-  </si>
-  <si>
-    <t>Di Ke Xiang Japanese Cake</t>
-  </si>
-  <si>
-    <t>Go bright sunflower cake</t>
-  </si>
-  <si>
-    <t>Rapeseed cake</t>
-  </si>
-  <si>
-    <t>Rapeseed meal</t>
-  </si>
-  <si>
-    <t>peanut cake</t>
-  </si>
-  <si>
-    <t>Corn germ cake</t>
-  </si>
-  <si>
-    <t>Rice bran cake</t>
-  </si>
-  <si>
-    <t>sesame cake</t>
-  </si>
-  <si>
-    <t>Tofu dregs</t>
-  </si>
-  <si>
-    <t>Corn meal residue</t>
-  </si>
-  <si>
-    <t>Potato flour residue</t>
-  </si>
-  <si>
-    <t>Pea flour residue</t>
-  </si>
-  <si>
-    <t>Mung bean flour residue</t>
-  </si>
-  <si>
-    <t>Tapioca flour residue</t>
-  </si>
-  <si>
-    <t>Soy sauce residue</t>
-  </si>
-  <si>
-    <t>corn trough</t>
-  </si>
-  <si>
-    <t>Sweet potato dry wine tank</t>
-  </si>
-  <si>
-    <t>Grain bran distiller's grains</t>
-  </si>
-  <si>
-    <t>Rice distiller's grains</t>
-  </si>
-  <si>
-    <t>Sorghum distiller's grains</t>
-  </si>
-  <si>
-    <t>Beer! Liquor lees</t>
-  </si>
-  <si>
-    <t>beet pulp</t>
-  </si>
-  <si>
-    <t>Orange pulp</t>
-  </si>
-  <si>
-    <t>Apple pomace</t>
-  </si>
-  <si>
-    <t>corn silage</t>
-  </si>
-  <si>
-    <t>Alfalfa silage</t>
-  </si>
-  <si>
-    <t>beet leaf silage</t>
-  </si>
-  <si>
-    <t>Leymus chinensis</t>
-  </si>
-  <si>
-    <t>alfalfa hay</t>
-  </si>
-  <si>
-    <t>wild hay</t>
-  </si>
-  <si>
-    <t>Alkali grass</t>
-  </si>
-  <si>
-    <t>Corn stalks</t>
-  </si>
-  <si>
-    <t>wheat straw</t>
-  </si>
-  <si>
-    <t>straw</t>
-  </si>
-  <si>
-    <t>cereal grass</t>
-  </si>
-  <si>
-    <t>sweet potato seedlings</t>
-  </si>
-  <si>
-    <t>peanut seedlings</t>
-  </si>
-  <si>
-    <t>大麦苗</t>
-  </si>
-  <si>
-    <t>甘薯藤</t>
-  </si>
-  <si>
-    <t>黑麦草</t>
-  </si>
-  <si>
-    <t>苜蓿</t>
-  </si>
-  <si>
-    <t>沙打旺</t>
-  </si>
-  <si>
-    <t>象草</t>
-  </si>
-  <si>
-    <t>野草</t>
-  </si>
-  <si>
-    <t>甘薯</t>
-  </si>
-  <si>
-    <t>胡萝卜</t>
-  </si>
-  <si>
-    <t>马铃薯</t>
-  </si>
-  <si>
-    <t>甜菜</t>
-  </si>
-  <si>
-    <t>甜菜丝干</t>
-  </si>
-  <si>
-    <t>芜菁甘蓝</t>
-  </si>
-  <si>
-    <t>玉米</t>
-  </si>
-  <si>
-    <t>高粱</t>
-  </si>
-  <si>
-    <t>大麦</t>
-  </si>
-  <si>
-    <t>籼稻谷</t>
-  </si>
-  <si>
-    <t>燕麦</t>
-  </si>
-  <si>
-    <t>小麦</t>
-  </si>
-  <si>
-    <t>油脂</t>
-  </si>
-  <si>
-    <t>小麦麸</t>
-  </si>
-  <si>
-    <t>玉米皮</t>
-  </si>
-  <si>
-    <t>米糠</t>
-  </si>
-  <si>
-    <t>高粱糠</t>
-  </si>
-  <si>
-    <t>次粉</t>
-  </si>
-  <si>
-    <t>大豆皮</t>
-  </si>
-  <si>
-    <t>豆饼</t>
-  </si>
-  <si>
-    <t>豆粕</t>
-  </si>
-  <si>
-    <t>红麻饼</t>
-  </si>
-  <si>
-    <t>郴籽饼</t>
-  </si>
-  <si>
-    <t>棉仁饼</t>
-  </si>
-  <si>
-    <t>棉仁柏</t>
-  </si>
-  <si>
-    <t>蒂壳向日资饼</t>
-  </si>
-  <si>
-    <t>去亮向日葵饼</t>
-  </si>
-  <si>
-    <t>菜籽饼</t>
-  </si>
-  <si>
-    <t>菜籽粕</t>
-  </si>
-  <si>
-    <t>花生饼</t>
-  </si>
-  <si>
-    <t>玉米胚芽饼</t>
-  </si>
-  <si>
-    <t>米糠饼</t>
-  </si>
-  <si>
-    <t>芝麻饼</t>
-  </si>
-  <si>
-    <t>豆腐渣</t>
-  </si>
-  <si>
-    <t>玉米粉渣</t>
-  </si>
-  <si>
-    <t>土豆粉渣</t>
-  </si>
-  <si>
-    <t>豌豆粉渣</t>
-  </si>
-  <si>
-    <t>绿豆粉渣</t>
-  </si>
-  <si>
-    <t>木薯粉渣</t>
-  </si>
-  <si>
-    <t>酱油渣</t>
-  </si>
-  <si>
-    <t>玉米酒槽</t>
-  </si>
-  <si>
-    <t>红薯干酒槽</t>
-  </si>
-  <si>
-    <t>谷糠酒糟</t>
-  </si>
-  <si>
-    <t>大米酒糟</t>
-  </si>
-  <si>
-    <t>高粱酒糟</t>
-  </si>
-  <si>
-    <t>啤!酒糟</t>
-  </si>
-  <si>
-    <t>甜菜渣</t>
-  </si>
-  <si>
-    <t>橘子渣</t>
-  </si>
-  <si>
-    <t>苹果渣</t>
-  </si>
-  <si>
-    <t>玉米青贮</t>
-  </si>
-  <si>
-    <t>苜蓿青贮</t>
-  </si>
-  <si>
-    <t>甜菜叶青贮</t>
-  </si>
-  <si>
-    <t>羊草</t>
-  </si>
-  <si>
-    <t>苜蓿干草</t>
-  </si>
-  <si>
-    <t>野干草</t>
-  </si>
-  <si>
-    <t>碱草</t>
-  </si>
-  <si>
-    <t>玉米秸秆</t>
-  </si>
-  <si>
-    <t>小麦秸秆</t>
-  </si>
-  <si>
-    <t>稻草</t>
-  </si>
-  <si>
-    <t>谷草</t>
-  </si>
-  <si>
-    <t>甘薯秧</t>
-  </si>
-  <si>
-    <t>花生秧</t>
-  </si>
-  <si>
-    <t>materia</t>
+    <t>Raw_materials</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Dry_matter</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Energy_Unit_RND</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Crude_protein</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>棉籽饼</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>cottonseed cake</t>
     <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
@@ -1413,7 +1415,7 @@
   <dimension ref="A1:H71"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1421,7 +1423,7 @@
     <col min="1" max="1" width="12.125" customWidth="1"/>
     <col min="2" max="2" width="8.5" style="3" customWidth="1"/>
     <col min="3" max="3" width="18.375" style="3" customWidth="1"/>
-    <col min="4" max="4" width="11" style="3" customWidth="1"/>
+    <col min="4" max="4" width="15.25" style="3" customWidth="1"/>
     <col min="5" max="5" width="7.25" style="3" customWidth="1"/>
     <col min="6" max="6" width="6.5" style="3" customWidth="1"/>
     <col min="7" max="7" width="11.5" style="3" customWidth="1"/>
@@ -1429,42 +1431,42 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>9</v>
-      </c>
       <c r="H1" s="1" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B2" s="2">
-        <v>15.7</v>
+        <v>0.157</v>
       </c>
       <c r="C2" s="2">
         <v>0.11</v>
       </c>
       <c r="D2" s="2">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="E2" s="2">
         <v>0.12</v>
@@ -1476,21 +1478,21 @@
         <v>38.909999999999997</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B3" s="2">
-        <v>13</v>
+        <v>0.13</v>
       </c>
       <c r="C3" s="2">
         <v>0.08</v>
       </c>
       <c r="D3" s="2">
-        <v>2.1</v>
+        <v>21</v>
       </c>
       <c r="E3" s="2">
         <v>0.2</v>
@@ -1502,21 +1504,21 @@
         <v>30.21</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B4" s="2">
-        <v>18</v>
+        <v>0.18</v>
       </c>
       <c r="C4" s="2">
         <v>0.14000000000000001</v>
       </c>
       <c r="D4" s="2">
-        <v>3.3</v>
+        <v>33</v>
       </c>
       <c r="E4" s="2">
         <v>0.13</v>
@@ -1528,21 +1530,21 @@
         <v>42.9</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B5" s="2">
-        <v>26.2</v>
+        <v>0.26200000000000001</v>
       </c>
       <c r="C5" s="2">
         <v>0.13</v>
       </c>
       <c r="D5" s="2">
-        <v>3.8</v>
+        <v>38</v>
       </c>
       <c r="E5" s="2">
         <v>0.34</v>
@@ -1554,21 +1556,21 @@
         <v>34.6</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B6" s="2">
-        <v>14.9</v>
+        <v>0.14899999999999999</v>
       </c>
       <c r="C6" s="2">
         <v>0.1</v>
       </c>
       <c r="D6" s="2">
-        <v>3.5</v>
+        <v>35</v>
       </c>
       <c r="E6" s="2">
         <v>0.2</v>
@@ -1580,21 +1582,21 @@
         <v>39.68</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B7" s="2">
-        <v>20</v>
+        <v>0.2</v>
       </c>
       <c r="C7" s="2">
         <v>0.13</v>
       </c>
       <c r="D7" s="2">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="E7" s="2">
         <v>0.15</v>
@@ -1606,21 +1608,21 @@
         <v>37.659999999999997</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B8" s="2">
-        <v>18.899999999999999</v>
+        <v>0.18899999999999997</v>
       </c>
       <c r="C8" s="2">
         <v>0.12</v>
       </c>
       <c r="D8" s="2">
-        <v>3.2</v>
+        <v>32</v>
       </c>
       <c r="E8" s="2">
         <v>0.24</v>
@@ -1632,21 +1634,21 @@
         <v>35.700000000000003</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B9" s="2">
-        <v>25</v>
+        <v>0.25</v>
       </c>
       <c r="C9" s="2">
         <v>0.26</v>
       </c>
       <c r="D9" s="2">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="E9" s="2">
         <v>0.13</v>
@@ -1658,21 +1660,21 @@
         <v>33.799999999999997</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B10" s="2">
-        <v>12</v>
+        <v>0.12</v>
       </c>
       <c r="C10" s="2">
         <v>0.13</v>
       </c>
       <c r="D10" s="2">
-        <v>0.3</v>
+        <v>3</v>
       </c>
       <c r="E10" s="2">
         <v>0.15</v>
@@ -1684,21 +1686,21 @@
         <v>55.69</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="B11" s="2">
-        <v>22</v>
+        <v>0.22</v>
       </c>
       <c r="C11" s="2">
         <v>0.23</v>
       </c>
       <c r="D11" s="2">
-        <v>1.6</v>
+        <v>16</v>
       </c>
       <c r="E11" s="2">
         <v>0.02</v>
@@ -1710,21 +1712,21 @@
         <v>55.69</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B12" s="2">
-        <v>15</v>
+        <v>0.15</v>
       </c>
       <c r="C12" s="2">
         <v>0.12</v>
       </c>
       <c r="D12" s="2">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="E12" s="2">
         <v>0.06</v>
@@ -1736,21 +1738,21 @@
         <v>46.71</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B13" s="2">
-        <v>88.6</v>
+        <v>0.8859999999999999</v>
       </c>
       <c r="C13" s="2">
         <v>0.8</v>
       </c>
       <c r="D13" s="2">
-        <v>7.3</v>
+        <v>73</v>
       </c>
       <c r="E13" s="2">
         <v>0.66</v>
@@ -1762,21 +1764,21 @@
         <v>32.700000000000003</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B14" s="2">
-        <v>10</v>
+        <v>0.1</v>
       </c>
       <c r="C14" s="2">
         <v>0.11</v>
       </c>
       <c r="D14" s="2">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="E14" s="2">
         <v>0.06</v>
@@ -1788,21 +1790,21 @@
         <v>33.869999999999997</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="B15" s="2">
-        <v>88.4</v>
+        <v>0.88400000000000001</v>
       </c>
       <c r="C15" s="2">
         <v>1</v>
       </c>
       <c r="D15" s="2">
-        <v>8.6</v>
+        <v>86</v>
       </c>
       <c r="E15" s="2">
         <v>0.08</v>
@@ -1814,21 +1816,21 @@
         <v>59.31</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B16" s="2">
-        <v>89.3</v>
+        <v>0.89300000000000002</v>
       </c>
       <c r="C16" s="2">
         <v>0.88</v>
       </c>
       <c r="D16" s="2">
-        <v>8.6999999999999993</v>
+        <v>87</v>
       </c>
       <c r="E16" s="2">
         <v>0.28999999999999998</v>
@@ -1840,21 +1842,21 @@
         <v>54.78</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B17" s="2">
-        <v>88.8</v>
+        <v>0.88800000000000001</v>
       </c>
       <c r="C17" s="2">
         <v>0.89</v>
       </c>
       <c r="D17" s="2">
-        <v>10.8</v>
+        <v>108.00000000000001</v>
       </c>
       <c r="E17" s="2">
         <v>0.28999999999999998</v>
@@ -1866,21 +1868,21 @@
         <v>54.3</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="B18" s="2">
-        <v>90.6</v>
+        <v>0.90599999999999992</v>
       </c>
       <c r="C18" s="2">
         <v>0.86</v>
       </c>
       <c r="D18" s="2">
-        <v>8.3000000000000007</v>
+        <v>83</v>
       </c>
       <c r="E18" s="2">
         <v>0.13</v>
@@ -1892,21 +1894,21 @@
         <v>18.940000000000001</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B19" s="2">
-        <v>90.3</v>
+        <v>0.90300000000000002</v>
       </c>
       <c r="C19" s="2">
         <v>0.86</v>
       </c>
       <c r="D19" s="2">
-        <v>11.6</v>
+        <v>115.99999999999999</v>
       </c>
       <c r="E19" s="2">
         <v>0.15</v>
@@ -1918,21 +1920,21 @@
         <v>53.18</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B20" s="2">
-        <v>91.8</v>
+        <v>0.91799999999999993</v>
       </c>
       <c r="C20" s="2">
         <v>1.03</v>
       </c>
       <c r="D20" s="2">
-        <v>12.1</v>
+        <v>121</v>
       </c>
       <c r="E20" s="2">
         <v>0.11</v>
@@ -1944,15 +1946,15 @@
         <v>55.55</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B21" s="2">
-        <v>99.5</v>
+        <v>0.995</v>
       </c>
       <c r="C21" s="2">
         <v>2.85</v>
@@ -1970,21 +1972,21 @@
         <v>0</v>
       </c>
       <c r="H21" s="1" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B22" s="2">
-        <v>88.6</v>
+        <v>0.8859999999999999</v>
       </c>
       <c r="C22" s="2">
         <v>0.73</v>
       </c>
       <c r="D22" s="2">
-        <v>14.4</v>
+        <v>144.00000000000003</v>
       </c>
       <c r="E22" s="2">
         <v>0.2</v>
@@ -1996,21 +1998,21 @@
         <v>52.9</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>99</v>
+        <v>93</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B23" s="2">
-        <v>87.9</v>
+        <v>0.879</v>
       </c>
       <c r="C23" s="2">
         <v>0.56999999999999995</v>
       </c>
       <c r="D23" s="2">
-        <v>10.199999999999999</v>
+        <v>102</v>
       </c>
       <c r="E23" s="2">
         <v>0.28000000000000003</v>
@@ -2022,21 +2024,21 @@
         <v>37.03</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B24" s="2">
-        <v>90.2</v>
+        <v>0.90200000000000002</v>
       </c>
       <c r="C24" s="2">
         <v>0.89</v>
       </c>
       <c r="D24" s="2">
-        <v>12.1</v>
+        <v>121</v>
       </c>
       <c r="E24" s="2">
         <v>0.14000000000000001</v>
@@ -2048,21 +2050,21 @@
         <v>55.3</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="B25" s="2">
-        <v>91.1</v>
+        <v>0.91099999999999992</v>
       </c>
       <c r="C25" s="2">
         <v>0.92</v>
       </c>
       <c r="D25" s="2">
-        <v>9.6</v>
+        <v>96</v>
       </c>
       <c r="E25" s="2">
         <v>7.0000000000000007E-2</v>
@@ -2074,21 +2076,21 @@
         <v>38.56</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="B26" s="2">
-        <v>87.2</v>
+        <v>0.872</v>
       </c>
       <c r="C26" s="2">
         <v>1</v>
       </c>
       <c r="D26" s="2">
-        <v>9.5</v>
+        <v>95</v>
       </c>
       <c r="E26" s="2">
         <v>0.08</v>
@@ -2100,21 +2102,21 @@
         <v>58.75</v>
       </c>
       <c r="H26" s="1" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B27" s="2">
-        <v>91</v>
+        <v>0.91</v>
       </c>
       <c r="C27" s="2">
         <v>0.67</v>
       </c>
       <c r="D27" s="2">
-        <v>18.8</v>
+        <v>188</v>
       </c>
       <c r="E27" s="2">
         <v>0.5</v>
@@ -2126,21 +2128,21 @@
         <v>40.72</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B28" s="2">
-        <v>91.1</v>
+        <v>0.91099999999999992</v>
       </c>
       <c r="C28" s="2">
         <v>0.97</v>
       </c>
       <c r="D28" s="2">
-        <v>37.4</v>
+        <v>374</v>
       </c>
       <c r="E28" s="2">
         <v>0.32</v>
@@ -2152,21 +2154,21 @@
         <v>59</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B29" s="2">
-        <v>89</v>
+        <v>0.89</v>
       </c>
       <c r="C29" s="2">
         <v>0.9</v>
       </c>
       <c r="D29" s="2">
-        <v>44.6</v>
+        <v>446</v>
       </c>
       <c r="E29" s="2">
         <v>0.3</v>
@@ -2178,21 +2180,21 @@
         <v>53.52</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B30" s="2">
-        <v>92</v>
+        <v>0.92</v>
       </c>
       <c r="C30" s="2">
         <v>0.91</v>
       </c>
       <c r="D30" s="2">
-        <v>33.1</v>
+        <v>331</v>
       </c>
       <c r="E30" s="2">
         <v>0.57999999999999996</v>
@@ -2204,21 +2206,21 @@
         <v>55.62</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>2</v>
+        <v>147</v>
+      </c>
+      <c r="B31" s="2">
+        <v>0.8909999999999999</v>
       </c>
       <c r="C31" s="2">
         <v>0.75</v>
       </c>
       <c r="D31" s="2">
-        <v>31.2</v>
+        <v>312</v>
       </c>
       <c r="E31" s="2">
         <v>0.52</v>
@@ -2230,21 +2232,21 @@
         <v>47.54</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>108</v>
+        <v>146</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B32" s="2">
-        <v>89.6</v>
+        <v>0.89599999999999991</v>
       </c>
       <c r="C32" s="2">
         <v>0.82</v>
       </c>
       <c r="D32" s="2">
-        <v>32.5</v>
+        <v>325</v>
       </c>
       <c r="E32" s="2">
         <v>0.27</v>
@@ -2256,21 +2258,21 @@
         <v>32.380000000000003</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="B33" s="2">
-        <v>91</v>
+        <v>0.91</v>
       </c>
       <c r="C33" s="2">
         <v>0.76</v>
       </c>
       <c r="D33" s="2">
-        <v>41.2</v>
+        <v>412.00000000000006</v>
       </c>
       <c r="E33" s="2">
         <v>0.17</v>
@@ -2282,21 +2284,21 @@
         <v>26.75</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="B34" s="2">
-        <v>92.9</v>
+        <v>0.92900000000000005</v>
       </c>
       <c r="C34" s="2">
         <v>0.45</v>
       </c>
       <c r="D34" s="2">
-        <v>24.8</v>
+        <v>248</v>
       </c>
       <c r="E34" s="2">
         <v>0.35</v>
@@ -2308,21 +2310,21 @@
         <v>40.049999999999997</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="B35" s="2">
-        <v>93.6</v>
+        <v>0.93599999999999994</v>
       </c>
       <c r="C35" s="2">
         <v>0.61</v>
       </c>
       <c r="D35" s="2">
-        <v>46.1</v>
+        <v>461</v>
       </c>
       <c r="E35" s="2">
         <v>0.53</v>
@@ -2334,21 +2336,21 @@
         <v>37.1</v>
       </c>
       <c r="H35" s="1" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="B36" s="2">
-        <v>92.4</v>
+        <v>0.92400000000000004</v>
       </c>
       <c r="C36" s="2">
         <v>0.84</v>
       </c>
       <c r="D36" s="2">
-        <v>36.200000000000003</v>
+        <v>362.00000000000006</v>
       </c>
       <c r="E36" s="2">
         <v>0.74</v>
@@ -2360,21 +2362,21 @@
         <v>40.5</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="B37" s="2">
-        <v>91</v>
+        <v>0.91</v>
       </c>
       <c r="C37" s="2">
         <v>0.67</v>
       </c>
       <c r="D37" s="2">
-        <v>37</v>
+        <v>370</v>
       </c>
       <c r="E37" s="2">
         <v>0.61</v>
@@ -2386,21 +2388,21 @@
         <v>37.869999999999997</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="B38" s="2">
-        <v>89</v>
+        <v>0.89</v>
       </c>
       <c r="C38" s="2">
         <v>0.91</v>
       </c>
       <c r="D38" s="2">
-        <v>46.4</v>
+        <v>463.99999999999994</v>
       </c>
       <c r="E38" s="2">
         <v>0.24</v>
@@ -2412,21 +2414,21 @@
         <v>57.36</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="B39" s="2">
-        <v>93</v>
+        <v>0.93</v>
       </c>
       <c r="C39" s="2">
         <v>0.93</v>
       </c>
       <c r="D39" s="2">
-        <v>17.5</v>
+        <v>175</v>
       </c>
       <c r="E39" s="2">
         <v>0.05</v>
@@ -2438,21 +2440,21 @@
         <v>54.3</v>
       </c>
       <c r="H39" s="1" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="B40" s="2">
-        <v>90.7</v>
+        <v>0.90700000000000003</v>
       </c>
       <c r="C40" s="2">
         <v>0.71</v>
       </c>
       <c r="D40" s="2">
-        <v>15.2</v>
+        <v>152</v>
       </c>
       <c r="E40" s="2">
         <v>0.2</v>
@@ -2464,21 +2466,21 @@
         <v>44.27</v>
       </c>
       <c r="H40" s="1" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="B41" s="2">
-        <v>92</v>
+        <v>0.92</v>
       </c>
       <c r="C41" s="2">
         <v>0.87</v>
       </c>
       <c r="D41" s="2">
-        <v>39.200000000000003</v>
+        <v>392</v>
       </c>
       <c r="E41" s="2">
         <v>2.2400000000000002</v>
@@ -2490,21 +2492,21 @@
         <v>52.97</v>
       </c>
       <c r="H41" s="1" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="B42" s="2">
-        <v>10.8</v>
+        <v>0.10800000000000001</v>
       </c>
       <c r="C42" s="2">
         <v>0.11</v>
       </c>
       <c r="D42" s="2">
-        <v>3.3</v>
+        <v>33</v>
       </c>
       <c r="E42" s="2">
         <v>0.05</v>
@@ -2516,21 +2518,21 @@
         <v>54.15</v>
       </c>
       <c r="H42" s="1" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="B43" s="2">
-        <v>15</v>
+        <v>0.15</v>
       </c>
       <c r="C43" s="2">
         <v>0.16</v>
       </c>
       <c r="D43" s="2">
-        <v>1.8</v>
+        <v>18.000000000000004</v>
       </c>
       <c r="E43" s="2">
         <v>0.02</v>
@@ -2542,21 +2544,21 @@
         <v>50</v>
       </c>
       <c r="H43" s="1" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="B44" s="2">
-        <v>15</v>
+        <v>0.15</v>
       </c>
       <c r="C44" s="2">
         <v>0.12</v>
       </c>
       <c r="D44" s="2">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="E44" s="2">
         <v>0.06</v>
@@ -2568,21 +2570,21 @@
         <v>43.79</v>
       </c>
       <c r="H44" s="1" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="B45" s="2">
-        <v>12</v>
+        <v>0.12</v>
       </c>
       <c r="C45" s="2">
         <v>0.09</v>
       </c>
       <c r="D45" s="2">
-        <v>2.5</v>
+        <v>25</v>
       </c>
       <c r="E45" s="2">
         <v>0.09</v>
@@ -2594,21 +2596,21 @@
         <v>38.979999999999997</v>
       </c>
       <c r="H45" s="1" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="B46" s="2">
-        <v>14</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="C46" s="2">
         <v>0.02</v>
       </c>
       <c r="D46" s="2">
-        <v>2.1</v>
+        <v>21</v>
       </c>
       <c r="E46" s="2">
         <v>0.06</v>
@@ -2620,21 +2622,21 @@
         <v>45.25</v>
       </c>
       <c r="H46" s="1" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="B47" s="2">
-        <v>91</v>
+        <v>0.91</v>
       </c>
       <c r="C47" s="2">
         <v>0.85</v>
       </c>
       <c r="D47" s="2">
-        <v>3</v>
+        <v>30</v>
       </c>
       <c r="E47" s="2">
         <v>0.32</v>
@@ -2646,21 +2648,21 @@
         <v>52.77</v>
       </c>
       <c r="H47" s="1" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="B48" s="2">
-        <v>23.4</v>
+        <v>0.23399999999999999</v>
       </c>
       <c r="C48" s="2">
         <v>0.21</v>
       </c>
       <c r="D48" s="2">
-        <v>7.1</v>
+        <v>71</v>
       </c>
       <c r="E48" s="2">
         <v>0.11</v>
@@ -2672,21 +2674,21 @@
         <v>61.9</v>
       </c>
       <c r="H48" s="1" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="B49" s="2">
-        <v>35</v>
+        <v>0.35</v>
       </c>
       <c r="C49" s="2">
         <v>0.26</v>
       </c>
       <c r="D49" s="2">
-        <v>6.4</v>
+        <v>64</v>
       </c>
       <c r="E49" s="2">
         <v>0.09</v>
@@ -2698,21 +2700,21 @@
         <v>53.11</v>
       </c>
       <c r="H49" s="1" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="B50" s="2">
-        <v>35</v>
+        <v>0.35</v>
       </c>
       <c r="C50" s="2">
         <v>0.18</v>
       </c>
       <c r="D50" s="2">
-        <v>5.7</v>
+        <v>57</v>
       </c>
       <c r="E50" s="2" t="s">
         <v>1</v>
@@ -2724,21 +2726,21 @@
         <v>28.4</v>
       </c>
       <c r="H50" s="1" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="B51" s="2">
-        <v>30</v>
+        <v>0.3</v>
       </c>
       <c r="C51" s="2">
         <v>0.11</v>
       </c>
       <c r="D51" s="2">
-        <v>3.8</v>
+        <v>38</v>
       </c>
       <c r="E51" s="2">
         <v>0.13</v>
@@ -2750,21 +2752,21 @@
         <v>20.88</v>
       </c>
       <c r="H51" s="1" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="B52" s="2">
-        <v>20.3</v>
+        <v>0.20300000000000001</v>
       </c>
       <c r="C52" s="2">
         <v>0.22</v>
       </c>
       <c r="D52" s="2">
-        <v>6</v>
+        <v>60</v>
       </c>
       <c r="E52" s="2">
         <v>0.16</v>
@@ -2776,21 +2778,21 @@
         <v>60.21</v>
       </c>
       <c r="H52" s="1" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="B53" s="2">
-        <v>37.700000000000003</v>
+        <v>0.377</v>
       </c>
       <c r="C53" s="2">
         <v>0.36</v>
       </c>
       <c r="D53" s="2">
-        <v>9.3000000000000007</v>
+        <v>93.000000000000014</v>
       </c>
       <c r="E53" s="2">
         <v>0.23</v>
@@ -2802,21 +2804,21 @@
         <v>53.11</v>
       </c>
       <c r="H53" s="1" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="B54" s="2">
-        <v>23.4</v>
+        <v>0.23399999999999999</v>
       </c>
       <c r="C54" s="2">
         <v>0.17</v>
       </c>
       <c r="D54" s="2">
-        <v>8.8000000000000007</v>
+        <v>88.000000000000014</v>
       </c>
       <c r="E54" s="2">
         <v>0.09</v>
@@ -2828,21 +2830,21 @@
         <v>42.08</v>
       </c>
       <c r="H54" s="1" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="B55" s="2">
-        <v>11.9</v>
+        <v>0.11900000000000001</v>
       </c>
       <c r="C55" s="2">
         <v>0.08</v>
       </c>
       <c r="D55" s="2">
-        <v>1.2</v>
+        <v>12</v>
       </c>
       <c r="E55" s="2">
         <v>0.1</v>
@@ -2854,21 +2856,21 @@
         <v>39.82</v>
       </c>
       <c r="H55" s="1" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="B56" s="2">
-        <v>89.2</v>
+        <v>0.89200000000000002</v>
       </c>
       <c r="C56" s="2">
         <v>0.81</v>
       </c>
       <c r="D56" s="2">
-        <v>5.6</v>
+        <v>55.999999999999993</v>
       </c>
       <c r="E56" s="2">
         <v>0.63</v>
@@ -2880,21 +2882,21 @@
         <v>51.37</v>
       </c>
       <c r="H56" s="1" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="B57" s="2">
-        <v>89</v>
+        <v>0.89</v>
       </c>
       <c r="C57" s="2">
         <v>0.68</v>
       </c>
       <c r="D57" s="2">
-        <v>4.5999999999999996</v>
+        <v>46</v>
       </c>
       <c r="E57" s="2">
         <v>0.45</v>
@@ -2906,21 +2908,21 @@
         <v>43.02</v>
       </c>
       <c r="H57" s="1" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="B58" s="2">
-        <v>22.7</v>
+        <v>0.22699999999999998</v>
       </c>
       <c r="C58" s="2">
         <v>0.12</v>
       </c>
       <c r="D58" s="2">
-        <v>1.6</v>
+        <v>16</v>
       </c>
       <c r="E58" s="2">
         <v>0.1</v>
@@ -2932,21 +2934,21 @@
         <v>31.6</v>
       </c>
       <c r="H58" s="1" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="B59" s="2">
-        <v>33.700000000000003</v>
+        <v>0.33700000000000002</v>
       </c>
       <c r="C59" s="2">
         <v>0.16</v>
       </c>
       <c r="D59" s="2">
-        <v>5.3</v>
+        <v>53</v>
       </c>
       <c r="E59" s="2">
         <v>0.5</v>
@@ -2958,21 +2960,21 @@
         <v>40.1</v>
       </c>
       <c r="H59" s="1" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="B60" s="2">
-        <v>37.5</v>
+        <v>0.375</v>
       </c>
       <c r="C60" s="2">
         <v>0.26</v>
       </c>
       <c r="D60" s="2">
-        <v>4.5999999999999996</v>
+        <v>46</v>
       </c>
       <c r="E60" s="2">
         <v>0.39</v>
@@ -2984,21 +2986,21 @@
         <v>34.5</v>
       </c>
       <c r="H60" s="1" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="B61" s="2">
-        <v>91.6</v>
+        <v>0.91599999999999993</v>
       </c>
       <c r="C61" s="2" t="s">
         <v>0</v>
       </c>
       <c r="D61" s="2">
-        <v>7.4</v>
+        <v>74.000000000000014</v>
       </c>
       <c r="E61" s="2">
         <v>0.37</v>
@@ -3010,21 +3012,21 @@
         <v>28.4</v>
       </c>
       <c r="H61" s="1" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="B62" s="2">
-        <v>92.4</v>
+        <v>0.92400000000000004</v>
       </c>
       <c r="C62" s="2">
         <v>0.56000000000000005</v>
       </c>
       <c r="D62" s="2">
-        <v>16.8</v>
+        <v>168</v>
       </c>
       <c r="E62" s="2">
         <v>1.95</v>
@@ -3036,21 +3038,21 @@
         <v>39.5</v>
       </c>
       <c r="H62" s="1" t="s">
-        <v>139</v>
+        <v>132</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="B63" s="2">
-        <v>87.9</v>
+        <v>0.879</v>
       </c>
       <c r="C63" s="2">
         <v>0.44</v>
       </c>
       <c r="D63" s="2">
-        <v>9.3000000000000007</v>
+        <v>93.000000000000014</v>
       </c>
       <c r="E63" s="2">
         <v>0.33</v>
@@ -3062,21 +3064,21 @@
         <v>32.700000000000003</v>
       </c>
       <c r="H63" s="1" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B64" s="2">
-        <v>87.8</v>
+        <v>0.878</v>
       </c>
       <c r="C64" s="2">
         <v>0.62</v>
       </c>
       <c r="D64" s="2">
-        <v>17</v>
+        <v>170</v>
       </c>
       <c r="E64" s="2">
         <v>0.39</v>
@@ -3088,21 +3090,21 @@
         <v>38.770000000000003</v>
       </c>
       <c r="H64" s="1" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="B65" s="2">
-        <v>91.7</v>
+        <v>0.91700000000000004</v>
       </c>
       <c r="C65" s="2">
         <v>0.28999999999999998</v>
       </c>
       <c r="D65" s="2">
-        <v>7.4</v>
+        <v>74.000000000000014</v>
       </c>
       <c r="E65" s="2">
         <v>0.42</v>
@@ -3114,21 +3116,21 @@
         <v>28.26</v>
       </c>
       <c r="H65" s="1" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="B66" s="2">
-        <v>90</v>
+        <v>0.9</v>
       </c>
       <c r="C66" s="2">
         <v>0.31</v>
       </c>
       <c r="D66" s="2">
-        <v>5.9</v>
+        <v>59.000000000000007</v>
       </c>
       <c r="E66" s="2">
         <v>0.39</v>
@@ -3140,21 +3142,21 @@
         <v>31.3</v>
       </c>
       <c r="H66" s="1" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="B67" s="2">
-        <v>89.6</v>
+        <v>0.89599999999999991</v>
       </c>
       <c r="C67" s="2">
         <v>0.24</v>
       </c>
       <c r="D67" s="2">
-        <v>5.6</v>
+        <v>55.999999999999993</v>
       </c>
       <c r="E67" s="2">
         <v>0.05</v>
@@ -3166,21 +3168,21 @@
         <v>21.02</v>
       </c>
       <c r="H67" s="1" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="B68" s="2">
-        <v>89.4</v>
+        <v>0.89400000000000002</v>
       </c>
       <c r="C68" s="2">
         <v>0.24</v>
       </c>
       <c r="D68" s="2">
-        <v>2.5</v>
+        <v>25</v>
       </c>
       <c r="E68" s="2">
         <v>7.0000000000000007E-2</v>
@@ -3192,21 +3194,21 @@
         <v>19.77</v>
       </c>
       <c r="H68" s="1" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="B69" s="2">
-        <v>90.7</v>
+        <v>0.90700000000000003</v>
       </c>
       <c r="C69" s="2">
         <v>0.34</v>
       </c>
       <c r="D69" s="2">
-        <v>4.5</v>
+        <v>45</v>
       </c>
       <c r="E69" s="2">
         <v>0.34</v>
@@ -3218,21 +3220,21 @@
         <v>27.84</v>
       </c>
       <c r="H69" s="1" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="B70" s="2">
-        <v>88</v>
+        <v>0.88</v>
       </c>
       <c r="C70" s="2">
         <v>0.41</v>
       </c>
       <c r="D70" s="2">
-        <v>8.1</v>
+        <v>81</v>
       </c>
       <c r="E70" s="2">
         <v>1.55</v>
@@ -3244,21 +3246,21 @@
         <v>35.4</v>
       </c>
       <c r="H70" s="1" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="B71" s="2">
-        <v>91.3</v>
+        <v>0.91299999999999992</v>
       </c>
       <c r="C71" s="2">
         <v>0.53</v>
       </c>
       <c r="D71" s="2">
-        <v>11</v>
+        <v>110</v>
       </c>
       <c r="E71" s="2">
         <v>1.29</v>
@@ -3270,7 +3272,7 @@
         <v>31.95</v>
       </c>
       <c r="H71" s="1" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
     </row>
   </sheetData>

</xml_diff>